<commit_message>
automatically backed up by learn
</commit_message>
<xml_diff>
--- a/NewSavedView.xlsx
+++ b/NewSavedView.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
+  <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="47">
   <si>
     <t>Unnamed: 0</t>
   </si>
@@ -46,71 +47,50 @@
     <t>business_id</t>
   </si>
   <si>
+    <t>cool</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>funny</t>
+  </si>
+  <si>
+    <t>review_id</t>
+  </si>
+  <si>
+    <t>stars</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>useful</t>
+  </si>
+  <si>
+    <t>user_id</t>
+  </si>
+  <si>
     <t>4JNXUYY8wbaaDmk3BPzlWw</t>
   </si>
   <si>
-    <t>cool</t>
-  </si>
-  <si>
-    <t>date</t>
-  </si>
-  <si>
     <t>2012-06-10</t>
   </si>
   <si>
-    <t>2012-01-20</t>
-  </si>
-  <si>
-    <t>2017-05-10</t>
-  </si>
-  <si>
-    <t>2014-05-03</t>
-  </si>
-  <si>
-    <t>2014-06-04</t>
-  </si>
-  <si>
-    <t>2017-07-23</t>
-  </si>
-  <si>
-    <t>2011-06-28</t>
-  </si>
-  <si>
-    <t>funny</t>
-  </si>
-  <si>
-    <t>review_id</t>
-  </si>
-  <si>
     <t>wl8BO_I-is-JaMwMW5c_gQ</t>
-  </si>
-  <si>
-    <t>cf9RrqHY9eQ9M53OPyXLtg</t>
-  </si>
-  <si>
-    <t>BvmhSQ6WFm2Jxu01G8OpdQ</t>
-  </si>
-  <si>
-    <t>IoKp9n1489XohTV_-EJ0IQ</t>
-  </si>
-  <si>
-    <t>7YNmSq7Lb1zi4SUKXaSjfg</t>
-  </si>
-  <si>
-    <t>sP5y4p1m-t5zYPeZ6_qRcA</t>
-  </si>
-  <si>
-    <t>gzBB-2e8fLOYFk997KnNvQ</t>
-  </si>
-  <si>
-    <t>stars</t>
-  </si>
-  <si>
-    <t>text</t>
   </si>
   <si>
     <t>I booked a table here for brunch and it did not disappoint, it was a great experience and more relaxed I feel that the pricy dinner menu would of been, with the same outdoor table overlooking the Bellagio fountains and the Paris hotel. Eggs Benedict for me was fab and some other good options on the menu. 
 I told them we were celebrating a birthday and got a chocolate cake with a candle brought out which I was pleased to find was not included on our bill at the end!</t>
+  </si>
+  <si>
+    <t>fo4mpUqgXL2mJqALc9AvbA</t>
+  </si>
+  <si>
+    <t>2012-01-20</t>
+  </si>
+  <si>
+    <t>cf9RrqHY9eQ9M53OPyXLtg</t>
   </si>
   <si>
     <t>Came here for lunch after a long night of partying.  I'm a huge fan of French food, and had definitely been craving it ever since I arrived at PH and saw that the Paris was next door.  Mon Ami Gabi definitely satisfied my craving!  A friend and I split the steak classique (steak with butter), and the quiche Lorraine.  So good!!!  The steak was perfectly cooked medium rare, as requested.  The quiche Lorraine was delicious, but I was so full by the time I got around to eating it that I only had a few bites; what I did eat was perfectly balanced.  My friends seemed to enjoy their orders as well.  I only wish that the restaurant served steak tartare... I would've been on that like white on rice!
@@ -118,10 +98,37 @@
 Definitely worth coming here for a meal that is nice, but not too nice (I'm looking at you, 16-course tasting menu at JG), when you're in Vegas.</t>
   </si>
   <si>
+    <t>TVvTtXwPXsvrg2KJGoOUTg</t>
+  </si>
+  <si>
+    <t>2017-05-10</t>
+  </si>
+  <si>
+    <t>BvmhSQ6WFm2Jxu01G8OpdQ</t>
+  </si>
+  <si>
     <t>Loved the fried goat cheese in tomato sauce along with dogfish 60 minutes IPA. Very nice view of the Vegas strip along with excellent service</t>
   </si>
   <si>
+    <t>etbAVunw-4kwr6VTRweZpA</t>
+  </si>
+  <si>
+    <t>2014-05-03</t>
+  </si>
+  <si>
+    <t>IoKp9n1489XohTV_-EJ0IQ</t>
+  </si>
+  <si>
     <t>Love the outdoor atmosphere. Price was right, service exceptional and the food tasted fantastic</t>
+  </si>
+  <si>
+    <t>vKXux2Xx3xcicTgYZoR0pg</t>
+  </si>
+  <si>
+    <t>2014-06-04</t>
+  </si>
+  <si>
+    <t>7YNmSq7Lb1zi4SUKXaSjfg</t>
   </si>
   <si>
     <t>Best steak in Vegas. Best mashed potatoes in Vegas. Best French restaurant in Vegas.
@@ -131,35 +138,29 @@
 They will definitely be seeing me again.</t>
   </si>
   <si>
+    <t>e3s1x4LLqfSkRTWDy_-Urg</t>
+  </si>
+  <si>
+    <t>2017-07-23</t>
+  </si>
+  <si>
+    <t>sP5y4p1m-t5zYPeZ6_qRcA</t>
+  </si>
+  <si>
     <t>Coming here for many years and this is my first bad experience. The food was still great, but the service and the new policy of not allowing you to have a sample tasting of wine before ordering , spoiled my excitement about eating here again. We like to try different wines and the server interaction and suggestions about wine was always a highlight of the meal.</t>
+  </si>
+  <si>
+    <t>CnhPN2j5hsM2gJ7UPmllFA</t>
+  </si>
+  <si>
+    <t>2011-06-28</t>
+  </si>
+  <si>
+    <t>gzBB-2e8fLOYFk997KnNvQ</t>
   </si>
   <si>
     <t>So disappointed.  There were five hostesses standing around as we showed up ten minutes early for our lunch reservation,. We were seated about 12 minutes after our requested time.  Once seated we waited forever for a server.  The entire experience was just SLOW.  My meal was just average, the salad was overdressed and we had to ask for water and more drinks.
 I was glad I did not suggest this restaurant since everyone in our group was let down</t>
-  </si>
-  <si>
-    <t>useful</t>
-  </si>
-  <si>
-    <t>user_id</t>
-  </si>
-  <si>
-    <t>fo4mpUqgXL2mJqALc9AvbA</t>
-  </si>
-  <si>
-    <t>TVvTtXwPXsvrg2KJGoOUTg</t>
-  </si>
-  <si>
-    <t>etbAVunw-4kwr6VTRweZpA</t>
-  </si>
-  <si>
-    <t>vKXux2Xx3xcicTgYZoR0pg</t>
-  </si>
-  <si>
-    <t>e3s1x4LLqfSkRTWDy_-Urg</t>
-  </si>
-  <si>
-    <t>CnhPN2j5hsM2gJ7UPmllFA</t>
   </si>
   <si>
     <t>Auxu_C_QmuyM_DW0jFK_hA</t>
@@ -169,26 +170,22 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -203,35 +200,26 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -519,12 +507,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:10">
       <c r="B1" s="1" t="s">
@@ -556,255 +550,255 @@
       </c>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" s="1">
+      <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>9</v>
       </c>
       <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
         <v>11</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>12</v>
       </c>
-      <c r="E2" t="s">
-        <v>20</v>
-      </c>
       <c r="F2" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="G2" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="H2" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="I2" t="s">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="J2" t="s">
-        <v>39</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:10">
-      <c r="A3" s="1">
+      <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3">
+        <v>18</v>
+      </c>
+      <c r="C3" t="n">
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3">
+        <v>19</v>
+      </c>
+      <c r="E3" t="n">
         <v>0</v>
       </c>
       <c r="F3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" t="n">
+        <v>4</v>
+      </c>
+      <c r="H3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" t="s">
         <v>22</v>
-      </c>
-      <c r="G3">
-        <v>4</v>
-      </c>
-      <c r="H3" t="s">
-        <v>31</v>
-      </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
-      <c r="J3" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="1">
+      <c r="A4" s="1" t="n">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4">
+        <v>18</v>
+      </c>
+      <c r="C4" t="n">
         <v>0</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4">
+        <v>23</v>
+      </c>
+      <c r="E4" t="n">
         <v>0</v>
       </c>
       <c r="F4" t="s">
-        <v>23</v>
-      </c>
-      <c r="G4">
+        <v>24</v>
+      </c>
+      <c r="G4" t="n">
         <v>4</v>
       </c>
       <c r="H4" t="s">
-        <v>32</v>
-      </c>
-      <c r="I4">
+        <v>25</v>
+      </c>
+      <c r="I4" t="n">
         <v>0</v>
       </c>
       <c r="J4" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="1">
+      <c r="A5" s="1" t="n">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5">
+        <v>18</v>
+      </c>
+      <c r="C5" t="n">
         <v>0</v>
       </c>
       <c r="D5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5">
+        <v>27</v>
+      </c>
+      <c r="E5" t="n">
         <v>0</v>
       </c>
       <c r="F5" t="s">
-        <v>24</v>
-      </c>
-      <c r="G5">
+        <v>28</v>
+      </c>
+      <c r="G5" t="n">
         <v>5</v>
       </c>
       <c r="H5" t="s">
-        <v>33</v>
-      </c>
-      <c r="I5">
+        <v>29</v>
+      </c>
+      <c r="I5" t="n">
         <v>0</v>
       </c>
       <c r="J5" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="1">
+      <c r="A6" s="1" t="n">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6">
+        <v>18</v>
+      </c>
+      <c r="C6" t="n">
         <v>0</v>
       </c>
       <c r="D6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6">
+        <v>31</v>
+      </c>
+      <c r="E6" t="n">
         <v>0</v>
       </c>
       <c r="F6" t="s">
-        <v>25</v>
-      </c>
-      <c r="G6">
+        <v>32</v>
+      </c>
+      <c r="G6" t="n">
         <v>5</v>
       </c>
       <c r="H6" t="s">
+        <v>33</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" t="s">
         <v>34</v>
-      </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-      <c r="J6" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="1">
+      <c r="A7" s="1" t="n">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7">
+        <v>18</v>
+      </c>
+      <c r="C7" t="n">
         <v>0</v>
       </c>
       <c r="D7" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7">
+        <v>35</v>
+      </c>
+      <c r="E7" t="n">
         <v>0</v>
       </c>
       <c r="F7" t="s">
-        <v>26</v>
-      </c>
-      <c r="G7">
+        <v>36</v>
+      </c>
+      <c r="G7" t="n">
         <v>5</v>
       </c>
       <c r="H7" t="s">
-        <v>35</v>
-      </c>
-      <c r="I7">
+        <v>37</v>
+      </c>
+      <c r="I7" t="n">
         <v>3</v>
       </c>
       <c r="J7" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="1">
+      <c r="A8" s="1" t="n">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8">
+        <v>18</v>
+      </c>
+      <c r="C8" t="n">
         <v>0</v>
       </c>
       <c r="D8" t="s">
-        <v>18</v>
-      </c>
-      <c r="E8">
+        <v>39</v>
+      </c>
+      <c r="E8" t="n">
         <v>0</v>
       </c>
       <c r="F8" t="s">
-        <v>27</v>
-      </c>
-      <c r="G8">
+        <v>40</v>
+      </c>
+      <c r="G8" t="n">
         <v>3</v>
       </c>
       <c r="H8" t="s">
-        <v>36</v>
-      </c>
-      <c r="I8">
+        <v>41</v>
+      </c>
+      <c r="I8" t="n">
         <v>0</v>
       </c>
       <c r="J8" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="1">
+      <c r="A9" s="1" t="n">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9">
+        <v>18</v>
+      </c>
+      <c r="C9" t="n">
         <v>0</v>
       </c>
       <c r="D9" t="s">
-        <v>19</v>
-      </c>
-      <c r="E9">
+        <v>43</v>
+      </c>
+      <c r="E9" t="n">
         <v>0</v>
       </c>
       <c r="F9" t="s">
-        <v>28</v>
-      </c>
-      <c r="G9">
+        <v>44</v>
+      </c>
+      <c r="G9" t="n">
         <v>2</v>
       </c>
       <c r="H9" t="s">
-        <v>37</v>
-      </c>
-      <c r="I9">
+        <v>45</v>
+      </c>
+      <c r="I9" t="n">
         <v>0</v>
       </c>
       <c r="J9" t="s">
@@ -812,6 +806,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>